<commit_message>
Modified template to take into account meeting 15.03.2013.
</commit_message>
<xml_diff>
--- a/Specification/SwVTD.xlsx
+++ b/Specification/SwVTD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="386" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="386" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Suivi Versions" sheetId="19" r:id="rId1"/>
@@ -114,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -187,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0">
+    <comment ref="G8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -211,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0">
+    <comment ref="I8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0">
+    <comment ref="F11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -355,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0">
+    <comment ref="F14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -379,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="G14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -403,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K14" authorId="0">
+    <comment ref="L14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1009,7 +1009,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="233">
   <si>
     <t>Test</t>
   </si>
@@ -1700,6 +1700,18 @@
   </si>
   <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>Raise Pantograph (file=SeqGlob.seq; arg1="test"; arg2=FileGlobals.cb1)</t>
+  </si>
+  <si>
+    <t>Check that Pantograph is lowered (type=YES_NO_TERMINATE; timeout=10000; default=2)</t>
+  </si>
+  <si>
+    <t>0,01 (tolerance=100; deviation=2; timeout=2500}</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -3253,8 +3265,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="33" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="34" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="35" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="33" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="34" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="35" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="34" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="35" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3262,13 +3325,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="46" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="37" xfId="46" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="46" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="47" xfId="46" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="46" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="48" xfId="46" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="46" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="46" applyBorder="1" applyAlignment="1">
@@ -3278,158 +3350,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="33" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="34" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="35" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="52" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="56" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="20" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="55" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="64" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="65" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="37" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="48" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="20" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="55" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="64" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="65" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="49" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="51" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="33" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="34" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="35" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="34" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="35" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="46" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="37" xfId="46" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="47" xfId="46" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="48" xfId="46" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="29" borderId="33" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3443,6 +3363,98 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="29" borderId="35" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="52" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="56" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="20" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="55" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="64" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="65" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="37" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="48" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="20" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="55" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="64" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="65" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="49" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="51" xfId="46" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="46" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
@@ -3510,7 +3522,24 @@
     <cellStyle name="Total 2" xfId="43"/>
     <cellStyle name="Vérification 2" xfId="44"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4284,16 +4313,16 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Style de tableau 1" pivot="0" count="1">
-      <tableStyleElement type="firstColumnStripe" dxfId="54"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="55"/>
     </tableStyle>
     <tableStyle name="tableau de Synthèse" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="53"/>
-      <tableStyleElement type="headerRow" dxfId="52"/>
+      <tableStyleElement type="wholeTable" dxfId="54"/>
+      <tableStyleElement type="headerRow" dxfId="53"/>
     </tableStyle>
     <tableStyle name="tableau de test" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="51"/>
-      <tableStyleElement type="headerRow" dxfId="50"/>
-      <tableStyleElement type="secondRowStripe" dxfId="49"/>
+      <tableStyleElement type="wholeTable" dxfId="52"/>
+      <tableStyleElement type="headerRow" dxfId="51"/>
+      <tableStyleElement type="secondRowStripe" dxfId="50"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -4602,49 +4631,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau44" displayName="Tableau44" ref="A1:D2" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau44" displayName="Tableau44" ref="A1:D2" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Version" dataDxfId="46"/>
-    <tableColumn id="2" name="Date" dataDxfId="45"/>
-    <tableColumn id="3" name="Nom" dataDxfId="44"/>
-    <tableColumn id="4" name="Modification" dataDxfId="43"/>
+    <tableColumn id="1" name="Version" dataDxfId="47"/>
+    <tableColumn id="2" name="Date" dataDxfId="46"/>
+    <tableColumn id="3" name="Nom" dataDxfId="45"/>
+    <tableColumn id="4" name="Modification" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="tableau de test" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:B12" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:B12" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:B12"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Codage" dataDxfId="1"/>
-    <tableColumn id="2" name="Désignation" dataDxfId="0"/>
+    <tableColumn id="1" name="Codage" dataDxfId="2"/>
+    <tableColumn id="2" name="Désignation" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau13" displayName="Tableau13" ref="A1:F14" headerRowDxfId="42" tableBorderDxfId="41" headerRowCellStyle="Normal 8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tableau13" displayName="Tableau13" ref="A1:F14" headerRowDxfId="43" tableBorderDxfId="42" headerRowCellStyle="Normal 8">
   <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Category" totalsRowLabel="Total" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="2" name="Test" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="3" name="Bench Conf" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="4" name="Associated requirement(s)" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="5" name="Description" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="6" name="Comment" totalsRowFunction="count" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="1" name="Category" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="2" name="Test" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="3" name="Bench Conf" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="4" name="Associated requirement(s)" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="5" name="Description" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="6" name="Comment" totalsRowFunction="count" dataDxfId="31" totalsRowDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="tableau de Synthèse" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau26" displayName="Tableau26" ref="B8:K21" headerRowDxfId="28">
-  <autoFilter ref="B8:K21"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau26" displayName="Tableau26" ref="B8:L21" headerRowDxfId="29">
+  <autoFilter ref="B8:L21"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="Target" totalsRowLabel="Total"/>
+    <tableColumn id="11" name="Comments" dataDxfId="0"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="3" name="Location"/>
     <tableColumn id="4" name="Type"/>
@@ -4660,11 +4690,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau3" displayName="Tableau3" ref="B23:K28" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tableau3" displayName="Tableau3" ref="B23:K28" totalsRowShown="0" headerRowDxfId="28">
   <autoFilter ref="B23:K28"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Target"/>
-    <tableColumn id="2" name="Path"/>
+    <tableColumn id="2" name="Comments"/>
     <tableColumn id="3" name="Location"/>
     <tableColumn id="4" name="Type"/>
     <tableColumn id="5" name="STEP 1"/>
@@ -4679,7 +4709,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau2615" displayName="Tableau2615" ref="B37:K50" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tableau2615" displayName="Tableau2615" ref="B37:K50" headerRowDxfId="27">
   <autoFilter ref="B37:K50"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Target" totalsRowLabel="Total"/>
@@ -4698,7 +4728,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau316" displayName="Tableau316" ref="B52:K57" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tableau316" displayName="Tableau316" ref="B52:K57" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="B52:K57"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Target"/>
@@ -4717,41 +4747,41 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau817" displayName="Tableau817" ref="B59:F62" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tableau817" displayName="Tableau817" ref="B59:F62" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="B59:F62"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Customized location alias" dataDxfId="22"/>
-    <tableColumn id="5" name="Unit" dataDxfId="21" dataCellStyle="Neutre"/>
-    <tableColumn id="4" name="Mode" dataDxfId="20" dataCellStyle="Neutre"/>
-    <tableColumn id="2" name="Location" dataDxfId="19"/>
-    <tableColumn id="3" name="Real location" dataDxfId="18"/>
+    <tableColumn id="1" name="Customized location alias" dataDxfId="23"/>
+    <tableColumn id="5" name="Unit" dataDxfId="22" dataCellStyle="Neutre"/>
+    <tableColumn id="4" name="Mode" dataDxfId="21" dataCellStyle="Neutre"/>
+    <tableColumn id="2" name="Location" dataDxfId="20"/>
+    <tableColumn id="3" name="Real location" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A37:B44" totalsRowShown="0" headerRowDxfId="17" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A37:B44" totalsRowShown="0" headerRowDxfId="18" headerRowCellStyle="Normal 2">
   <autoFilter ref="A37:B44"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Section name" dataDxfId="16" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" name="Section code" dataDxfId="15" dataCellStyle="Normal 2"/>
+    <tableColumn id="1" name="Section name" dataDxfId="17" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" name="Section code" dataDxfId="16" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A4:G9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A4:G9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
   <autoFilter ref="A4:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Conf" dataDxfId="12" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" name="Sections" dataDxfId="11" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" name="Colonne1" dataDxfId="10" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" name="Colonne2" dataDxfId="9" dataCellStyle="Normal 2"/>
-    <tableColumn id="5" name="Colonne3" dataDxfId="8" dataCellStyle="Normal 2"/>
-    <tableColumn id="6" name="Colonne4" dataDxfId="7" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" name="Colonne5" dataDxfId="6" dataCellStyle="Normal 2"/>
+    <tableColumn id="1" name="Conf" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" name="Sections" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" name="Colonne1" dataDxfId="11" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" name="Colonne2" dataDxfId="10" dataCellStyle="Normal 2"/>
+    <tableColumn id="5" name="Colonne3" dataDxfId="9" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" name="Colonne4" dataDxfId="8" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" name="Colonne5" dataDxfId="7" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5771,380 +5801,380 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
-      <c r="B2" s="144" t="str">
+      <c r="B2" s="97" t="str">
         <f>D4&amp;" "&amp;D5&amp;" - "&amp;D3</f>
         <v>B2_037_1 A1
 A1
 A1 - TFE-AHT-F11</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145"/>
-      <c r="J2" s="145"/>
-      <c r="K2" s="145"/>
-      <c r="L2" s="145"/>
-      <c r="M2" s="145"/>
-      <c r="N2" s="146"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="99"/>
       <c r="O2" s="22"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22"/>
-      <c r="B3" s="162" t="s">
+      <c r="B3" s="126" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="163"/>
-      <c r="D3" s="152" t="s">
+      <c r="C3" s="127"/>
+      <c r="D3" s="108" t="s">
         <v>151</v>
       </c>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
-      <c r="J3" s="153"/>
-      <c r="K3" s="153"/>
-      <c r="L3" s="153"/>
-      <c r="M3" s="153"/>
-      <c r="N3" s="154"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="110"/>
       <c r="O3" s="22"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="164" t="s">
+      <c r="B4" s="128" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="165"/>
-      <c r="D4" s="155" t="s">
+      <c r="C4" s="129"/>
+      <c r="D4" s="111" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="156"/>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156"/>
-      <c r="H4" s="156"/>
-      <c r="I4" s="156"/>
-      <c r="J4" s="156"/>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156"/>
-      <c r="M4" s="156"/>
-      <c r="N4" s="157"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="113"/>
       <c r="O4" s="22"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="130" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="167"/>
-      <c r="D5" s="158" t="s">
+      <c r="C5" s="131"/>
+      <c r="D5" s="114" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="99"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="116"/>
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="166" t="s">
+      <c r="B6" s="130" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="167"/>
-      <c r="D6" s="159">
+      <c r="C6" s="131"/>
+      <c r="D6" s="117">
         <v>41040</v>
       </c>
-      <c r="E6" s="160"/>
-      <c r="F6" s="160"/>
-      <c r="G6" s="160"/>
-      <c r="H6" s="160"/>
-      <c r="I6" s="160"/>
-      <c r="J6" s="160"/>
-      <c r="K6" s="160"/>
-      <c r="L6" s="160"/>
-      <c r="M6" s="160"/>
-      <c r="N6" s="161"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="118"/>
+      <c r="M6" s="118"/>
+      <c r="N6" s="119"/>
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
-      <c r="B7" s="166" t="s">
+      <c r="B7" s="130" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="167"/>
-      <c r="D7" s="103" t="s">
+      <c r="C7" s="131"/>
+      <c r="D7" s="123" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="104"/>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
-      <c r="K7" s="104"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="105"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="125"/>
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
-      <c r="B8" s="112" t="s">
+      <c r="B8" s="152" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="113"/>
-      <c r="D8" s="106" t="s">
+      <c r="C8" s="153"/>
+      <c r="D8" s="120" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
-      <c r="K8" s="107"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="107"/>
-      <c r="N8" s="108"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="121"/>
+      <c r="M8" s="121"/>
+      <c r="N8" s="122"/>
       <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
-      <c r="B9" s="114" t="s">
+      <c r="B9" s="154" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="115"/>
-      <c r="D9" s="100" t="s">
+      <c r="C9" s="155"/>
+      <c r="D9" s="166" t="s">
         <v>141</v>
       </c>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="102"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="167"/>
+      <c r="G9" s="167"/>
+      <c r="H9" s="167"/>
+      <c r="I9" s="167"/>
+      <c r="J9" s="167"/>
+      <c r="K9" s="167"/>
+      <c r="L9" s="167"/>
+      <c r="M9" s="167"/>
+      <c r="N9" s="168"/>
       <c r="O9" s="22"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
-      <c r="B10" s="116" t="s">
+      <c r="B10" s="156" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="117"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="98"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
-      <c r="L10" s="98"/>
-      <c r="M10" s="98"/>
-      <c r="N10" s="99"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="169"/>
+      <c r="E10" s="115"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="115"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="115"/>
+      <c r="M10" s="115"/>
+      <c r="N10" s="116"/>
       <c r="O10" s="22"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
-      <c r="B11" s="116" t="s">
+      <c r="B11" s="156" t="s">
         <v>145</v>
       </c>
-      <c r="C11" s="117"/>
-      <c r="D11" s="97"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="98"/>
-      <c r="M11" s="98"/>
-      <c r="N11" s="99"/>
+      <c r="C11" s="157"/>
+      <c r="D11" s="169"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="115"/>
+      <c r="K11" s="115"/>
+      <c r="L11" s="115"/>
+      <c r="M11" s="115"/>
+      <c r="N11" s="116"/>
       <c r="O11" s="22"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="158" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="119"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="101"/>
-      <c r="M12" s="101"/>
-      <c r="N12" s="102"/>
+      <c r="C12" s="159"/>
+      <c r="D12" s="166"/>
+      <c r="E12" s="167"/>
+      <c r="F12" s="167"/>
+      <c r="G12" s="167"/>
+      <c r="H12" s="167"/>
+      <c r="I12" s="167"/>
+      <c r="J12" s="167"/>
+      <c r="K12" s="167"/>
+      <c r="L12" s="167"/>
+      <c r="M12" s="167"/>
+      <c r="N12" s="168"/>
       <c r="O12" s="22"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="158" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="119"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="104"/>
-      <c r="N13" s="105"/>
+      <c r="C13" s="159"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="124"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="124"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="124"/>
+      <c r="M13" s="124"/>
+      <c r="N13" s="125"/>
       <c r="O13" s="22"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="158" t="s">
         <v>148</v>
       </c>
-      <c r="C14" s="119"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="104"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="105"/>
+      <c r="C14" s="159"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="124"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="124"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="124"/>
+      <c r="N14" s="125"/>
       <c r="O14" s="22"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="120" t="s">
+      <c r="B15" s="160" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="121"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="98"/>
-      <c r="L15" s="98"/>
-      <c r="M15" s="98"/>
-      <c r="N15" s="99"/>
+      <c r="C15" s="161"/>
+      <c r="D15" s="169"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="115"/>
+      <c r="L15" s="115"/>
+      <c r="M15" s="115"/>
+      <c r="N15" s="116"/>
       <c r="O15" s="22"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="118" t="s">
+      <c r="B16" s="158" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="119"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="101"/>
-      <c r="N16" s="102"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="166"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="167"/>
+      <c r="G16" s="167"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="167"/>
+      <c r="J16" s="167"/>
+      <c r="K16" s="167"/>
+      <c r="L16" s="167"/>
+      <c r="M16" s="167"/>
+      <c r="N16" s="168"/>
       <c r="O16" s="22"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="114" t="s">
+      <c r="B17" s="154" t="s">
         <v>154</v>
       </c>
-      <c r="C17" s="115"/>
-      <c r="D17" s="103"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="104"/>
-      <c r="I17" s="104"/>
-      <c r="J17" s="104"/>
-      <c r="K17" s="104"/>
-      <c r="L17" s="104"/>
-      <c r="M17" s="104"/>
-      <c r="N17" s="105"/>
+      <c r="C17" s="155"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="124"/>
+      <c r="H17" s="124"/>
+      <c r="I17" s="124"/>
+      <c r="J17" s="124"/>
+      <c r="K17" s="124"/>
+      <c r="L17" s="124"/>
+      <c r="M17" s="124"/>
+      <c r="N17" s="125"/>
       <c r="O17" s="22"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="162" t="s">
         <v>152</v>
       </c>
-      <c r="C18" s="123"/>
-      <c r="D18" s="103"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="104"/>
-      <c r="I18" s="104"/>
-      <c r="J18" s="104"/>
-      <c r="K18" s="104"/>
-      <c r="L18" s="104"/>
-      <c r="M18" s="104"/>
-      <c r="N18" s="105"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="124"/>
+      <c r="J18" s="124"/>
+      <c r="K18" s="124"/>
+      <c r="L18" s="124"/>
+      <c r="M18" s="124"/>
+      <c r="N18" s="125"/>
       <c r="O18" s="22"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
-      <c r="B19" s="124" t="s">
+      <c r="B19" s="164" t="s">
         <v>155</v>
       </c>
-      <c r="C19" s="125"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="107"/>
-      <c r="H19" s="107"/>
-      <c r="I19" s="107"/>
-      <c r="J19" s="107"/>
-      <c r="K19" s="107"/>
-      <c r="L19" s="107"/>
-      <c r="M19" s="107"/>
-      <c r="N19" s="108"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="121"/>
+      <c r="F19" s="121"/>
+      <c r="G19" s="121"/>
+      <c r="H19" s="121"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="121"/>
+      <c r="K19" s="121"/>
+      <c r="L19" s="121"/>
+      <c r="M19" s="121"/>
+      <c r="N19" s="122"/>
       <c r="O19" s="22"/>
     </row>
     <row r="20" spans="1:15" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
-      <c r="B20" s="168" t="s">
+      <c r="B20" s="132" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="169"/>
-      <c r="D20" s="147"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="148"/>
-      <c r="G20" s="148"/>
-      <c r="H20" s="148"/>
-      <c r="I20" s="148"/>
-      <c r="J20" s="148"/>
-      <c r="K20" s="148"/>
-      <c r="L20" s="148"/>
-      <c r="M20" s="148"/>
-      <c r="N20" s="149"/>
+      <c r="C20" s="133"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="101"/>
+      <c r="I20" s="101"/>
+      <c r="J20" s="101"/>
+      <c r="K20" s="101"/>
+      <c r="L20" s="101"/>
+      <c r="M20" s="101"/>
+      <c r="N20" s="102"/>
       <c r="O20" s="22"/>
     </row>
     <row r="21" spans="1:15" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6166,27 +6196,27 @@
     </row>
     <row r="22" spans="1:15" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="103" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="111"/>
-      <c r="F22" s="109" t="s">
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="G22" s="110"/>
-      <c r="H22" s="111"/>
-      <c r="I22" s="109" t="s">
+      <c r="G22" s="104"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="103" t="s">
         <v>107</v>
       </c>
-      <c r="J22" s="110"/>
-      <c r="K22" s="111"/>
-      <c r="L22" s="109" t="s">
+      <c r="J22" s="104"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="103" t="s">
         <v>108</v>
       </c>
-      <c r="M22" s="150"/>
-      <c r="N22" s="151"/>
+      <c r="M22" s="106"/>
+      <c r="N22" s="107"/>
       <c r="O22" s="22"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -6200,18 +6230,18 @@
       <c r="F23" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="G23" s="136"/>
-      <c r="H23" s="137"/>
+      <c r="G23" s="144"/>
+      <c r="H23" s="145"/>
       <c r="I23" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="J23" s="136"/>
-      <c r="K23" s="137"/>
+      <c r="J23" s="144"/>
+      <c r="K23" s="145"/>
       <c r="L23" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="M23" s="130"/>
-      <c r="N23" s="131"/>
+      <c r="M23" s="146"/>
+      <c r="N23" s="147"/>
       <c r="O23" s="22"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -6225,18 +6255,18 @@
       <c r="F24" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="126"/>
-      <c r="H24" s="127"/>
+      <c r="G24" s="134"/>
+      <c r="H24" s="135"/>
       <c r="I24" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="J24" s="126"/>
-      <c r="K24" s="127"/>
+      <c r="J24" s="134"/>
+      <c r="K24" s="135"/>
       <c r="L24" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="M24" s="132"/>
-      <c r="N24" s="133"/>
+      <c r="M24" s="148"/>
+      <c r="N24" s="149"/>
       <c r="O24" s="22"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -6244,24 +6274,24 @@
       <c r="B25" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="126"/>
-      <c r="D25" s="126"/>
-      <c r="E25" s="127"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="135"/>
       <c r="F25" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="126"/>
-      <c r="H25" s="127"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="135"/>
       <c r="I25" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="J25" s="126"/>
-      <c r="K25" s="127"/>
+      <c r="J25" s="134"/>
+      <c r="K25" s="135"/>
       <c r="L25" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="M25" s="132"/>
-      <c r="N25" s="133"/>
+      <c r="M25" s="148"/>
+      <c r="N25" s="149"/>
       <c r="O25" s="22"/>
     </row>
     <row r="26" spans="1:15" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6275,18 +6305,18 @@
       <c r="F26" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="G26" s="128"/>
-      <c r="H26" s="129"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="137"/>
       <c r="I26" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="J26" s="128"/>
-      <c r="K26" s="129"/>
+      <c r="J26" s="136"/>
+      <c r="K26" s="137"/>
       <c r="L26" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="M26" s="134"/>
-      <c r="N26" s="135"/>
+      <c r="M26" s="150"/>
+      <c r="N26" s="151"/>
       <c r="O26" s="22"/>
     </row>
     <row r="27" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6308,6 +6338,47 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="D11:N11"/>
+    <mergeCell ref="D12:N12"/>
+    <mergeCell ref="D13:N13"/>
+    <mergeCell ref="D19:N19"/>
+    <mergeCell ref="D14:N14"/>
+    <mergeCell ref="D15:N15"/>
+    <mergeCell ref="D16:N16"/>
+    <mergeCell ref="D17:N17"/>
+    <mergeCell ref="D18:N18"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D9:N9"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="D20:N20"/>
     <mergeCell ref="I22:K22"/>
@@ -6324,47 +6395,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D9:N9"/>
-    <mergeCell ref="D10:N10"/>
-    <mergeCell ref="D11:N11"/>
-    <mergeCell ref="D12:N12"/>
-    <mergeCell ref="D13:N13"/>
-    <mergeCell ref="D19:N19"/>
-    <mergeCell ref="D14:N14"/>
-    <mergeCell ref="D15:N15"/>
-    <mergeCell ref="D16:N16"/>
-    <mergeCell ref="D17:N17"/>
-    <mergeCell ref="D18:N18"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -6645,8 +6675,8 @@
   </sheetPr>
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -6671,24 +6701,25 @@
     <col min="18" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="84" t="s">
         <v>226</v>
       </c>
       <c r="C1" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="D1" s="85"/>
+      <c r="F1" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="71"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" collapsed="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="68"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="71"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D2" s="87"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -6697,59 +6728,59 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" hidden="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="67" t="s">
+    <row r="3" spans="1:12" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="65"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="89"/>
-    </row>
-    <row r="4" spans="1:11" ht="16.5" hidden="1" outlineLevel="2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="27" t="s">
+      <c r="G3" s="65"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="89"/>
+    </row>
+    <row r="4" spans="1:12" ht="16.5" outlineLevel="2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="91"/>
-    </row>
-    <row r="5" spans="1:11" ht="27" hidden="1" outlineLevel="2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="27" t="s">
+      <c r="G4" s="65"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="91"/>
+    </row>
+    <row r="5" spans="1:12" ht="27" outlineLevel="2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="F5" s="65" t="s">
+      <c r="G5" s="65" t="s">
         <v>165</v>
       </c>
-      <c r="G5" s="90" t="s">
+      <c r="H5" s="90" t="s">
         <v>166</v>
       </c>
-      <c r="H5" s="66" t="s">
+      <c r="I5" s="66" t="s">
         <v>167</v>
       </c>
-      <c r="I5" s="90" t="s">
+      <c r="J5" s="90" t="s">
         <v>168</v>
       </c>
-      <c r="J5" s="65"/>
-      <c r="K5" s="91"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.5" hidden="1" outlineLevel="2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="27" t="s">
+      <c r="K5" s="65"/>
+      <c r="L5" s="91"/>
+    </row>
+    <row r="6" spans="1:12" ht="16.5" outlineLevel="2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="91"/>
-    </row>
-    <row r="7" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="G6" s="65"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="91"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E7" s="87"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -6758,291 +6789,298 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="92"/>
       <c r="B8" s="93" t="s">
         <v>60</v>
       </c>
       <c r="C8" s="93" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="D8" s="93" t="s">
+      <c r="E8" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="93" t="s">
+      <c r="F8" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="F8" s="93" t="s">
+      <c r="G8" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="G8" s="93" t="s">
+      <c r="H8" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="H8" s="93" t="s">
+      <c r="I8" s="93" t="s">
         <v>173</v>
       </c>
-      <c r="I8" s="93" t="s">
+      <c r="J8" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="93" t="s">
+      <c r="K8" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="93" t="s">
+      <c r="L8" s="93" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="170" t="s">
         <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>0</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="171"/>
       <c r="B10" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>10</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>10</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="171"/>
       <c r="B11" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>1</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="171"/>
       <c r="B12" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>1</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="171"/>
       <c r="B13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>1</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="171"/>
       <c r="B14" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="171"/>
       <c r="B15" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>0</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="171"/>
       <c r="B16" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>0</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="171"/>
       <c r="B17" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>1.6</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="171"/>
       <c r="B18" s="94" t="s">
         <v>207</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="C18" s="94"/>
+      <c r="G18" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="171"/>
       <c r="B19" s="94" t="s">
         <v>208</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="C19" s="94"/>
+      <c r="G19" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B20" s="94" t="s">
         <v>210</v>
       </c>
-      <c r="G20" s="1">
+      <c r="C20" s="94"/>
+      <c r="H20" s="1">
         <v>7000</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B21" s="94" t="s">
         <v>211</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="94"/>
+      <c r="I21" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B22" s="94"/>
     </row>
-    <row r="23" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B23" s="93" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="93" t="s">
-        <v>169</v>
+        <v>232</v>
       </c>
       <c r="D23" s="93" t="s">
         <v>61</v>
@@ -7069,7 +7107,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="172" t="s">
         <v>62</v>
       </c>
@@ -7101,7 +7139,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="172"/>
       <c r="B25" s="1" t="s">
         <v>217</v>
@@ -7116,13 +7154,13 @@
         <v>206</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="172"/>
       <c r="B26" s="1" t="s">
         <v>220</v>
@@ -7144,7 +7182,7 @@
       </c>
       <c r="M26" s="10"/>
     </row>
-    <row r="27" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="172"/>
       <c r="B27" s="1" t="s">
         <v>224</v>
@@ -7162,16 +7200,16 @@
         <v>219</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="172"/>
       <c r="B28" s="94" t="s">
         <v>208</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="84" t="s">
         <v>227</v>
@@ -7703,8 +7741,8 @@
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange password="D262" sqref="E1:K2 E30:K31" name="Plage1_5"/>
-    <protectedRange password="D262" sqref="E3:K4 E32:K33" name="Plage1_7"/>
+    <protectedRange password="D262" sqref="F1:L1 E30:K31 E2:K2" name="Plage1_5"/>
+    <protectedRange password="D262" sqref="F3:L4 E32:K33" name="Plage1_7"/>
   </protectedRanges>
   <mergeCells count="2">
     <mergeCell ref="A9:A19"/>
@@ -7750,7 +7788,7 @@
   <sheetPr codeName="Feuil7"/>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>